<commit_message>
back testing and analyzing trends
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Flatiron\Capstone\sports_predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04AE447-A6F8-4648-A425-EB076E16BD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C60A6E-E4D3-4999-B7CA-3D6BAC364A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{DD114168-415D-4080-8C71-BE6BCC24E486}"/>
+    <workbookView xWindow="1830" yWindow="3195" windowWidth="21600" windowHeight="11835" xr2:uid="{DD114168-415D-4080-8C71-BE6BCC24E486}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,19 +130,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -159,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,30 +176,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D21BD6-6A32-417D-9AE2-A89192511320}">
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,277 +632,93 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>108.5</v>
+        <v>110.1</v>
       </c>
       <c r="B2" s="1">
-        <v>103.5</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1">
-        <v>0.55300000000000005</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="D2" s="1">
-        <v>0.23599999999999999</v>
+        <v>0.24399999999999999</v>
       </c>
       <c r="E2" s="1">
-        <v>16.5</v>
+        <v>25.9</v>
       </c>
       <c r="F2" s="1">
-        <v>78</v>
+        <v>80.3</v>
       </c>
       <c r="G2" s="1">
-        <v>63.6</v>
+        <v>58.9</v>
       </c>
       <c r="H2" s="1">
-        <v>6.6</v>
+        <v>7.6</v>
       </c>
       <c r="I2" s="1">
-        <v>5.2</v>
+        <v>2.6</v>
       </c>
       <c r="J2" s="1">
-        <v>14.1</v>
+        <v>13.7</v>
       </c>
       <c r="K2" s="1">
-        <v>109.1</v>
+        <v>111.5</v>
       </c>
       <c r="L2" s="1">
-        <v>104.1</v>
+        <v>104.3</v>
       </c>
       <c r="M2" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1">
-        <v>0.67</v>
+        <v>0.8</v>
       </c>
       <c r="O2" s="1">
-        <v>115.1</v>
+        <v>102</v>
       </c>
       <c r="P2" s="1">
-        <v>101.8</v>
+        <v>111.3</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.55400000000000005</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="R2" s="1">
-        <v>0.23200000000000001</v>
+        <v>0.221</v>
       </c>
       <c r="S2" s="1">
-        <v>23</v>
+        <v>25.2</v>
       </c>
       <c r="T2" s="1">
-        <v>82.1</v>
+        <v>78.5</v>
       </c>
       <c r="U2" s="1">
-        <v>70.599999999999994</v>
+        <v>63.1</v>
       </c>
       <c r="V2" s="1">
-        <v>10.6</v>
+        <v>7</v>
       </c>
       <c r="W2" s="1">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="X2" s="1">
         <v>13.8</v>
       </c>
       <c r="Y2" s="1">
-        <v>112.6</v>
+        <v>104.4</v>
       </c>
       <c r="Z2" s="1">
-        <v>99.6</v>
+        <v>113.9</v>
       </c>
       <c r="AA2" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AB2" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>110.2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>103.5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.53300000000000003</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="E3" s="2">
-        <v>24.8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>78.3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>52.2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2">
-        <v>5</v>
-      </c>
-      <c r="J3" s="2">
-        <v>13.7</v>
-      </c>
-      <c r="K3" s="2">
-        <v>112.2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>105.5</v>
-      </c>
-      <c r="M3" s="2">
-        <v>6</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="O3" s="2">
-        <v>109.9</v>
-      </c>
-      <c r="P3" s="2">
-        <v>105.7</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="S3" s="2">
-        <v>22.1</v>
-      </c>
-      <c r="T3" s="2">
-        <v>72.8</v>
-      </c>
-      <c r="U3" s="2">
-        <v>57</v>
-      </c>
-      <c r="V3" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="W3" s="2">
-        <v>5.9</v>
-      </c>
-      <c r="X3" s="2">
-        <v>11.9</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>115.1</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>110.8</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>6</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>10</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>108.5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>103.3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.43</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="E4" s="2">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="F4" s="2">
-        <v>76</v>
-      </c>
-      <c r="G4" s="2">
-        <v>59.2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>9.1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>5</v>
-      </c>
-      <c r="J4" s="2">
-        <v>12.7</v>
-      </c>
-      <c r="K4" s="2">
-        <v>107.6</v>
-      </c>
-      <c r="L4" s="2">
-        <v>102.4</v>
-      </c>
-      <c r="M4" s="2">
-        <v>9</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="O4" s="2">
-        <v>109.6</v>
-      </c>
-      <c r="P4" s="2">
-        <v>109.5</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.188</v>
-      </c>
-      <c r="S4" s="2">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="T4" s="2">
-        <v>77.400000000000006</v>
-      </c>
-      <c r="U4" s="2">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="V4" s="2">
-        <v>8.9</v>
-      </c>
-      <c r="W4" s="2">
-        <v>5.2</v>
-      </c>
-      <c r="X4" s="2">
-        <v>11.6</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>107.2</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>107.1</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>7</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0.28571428570000001</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="AD4" s="3">
+        <v>0.14285714290000001</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="AD2" s="1">
         <v>2021</v>
       </c>
     </row>

</xml_diff>